<commit_message>
large update in CO2 price project
</commit_message>
<xml_diff>
--- a/projects/CO2Price/data/rawData/Mappings.xlsx
+++ b/projects/CO2Price/data/rawData/Mappings.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sxj477\Documents\GitHub\CGE_Generator\projects\CO2Price\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sxj477\Documents\GitHub\CGE_Generator\projects\CO2Price\data\rawData\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="147">
   <si>
     <t>inv7toinvGR/n</t>
   </si>
@@ -459,6 +459,12 @@
   </si>
   <si>
     <t>97000_</t>
+  </si>
+  <si>
+    <t>s69tosFull/s</t>
+  </si>
+  <si>
+    <t>s69tosFull/ss</t>
   </si>
 </sst>
 </file>
@@ -805,23 +811,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F70"/>
+  <dimension ref="A1:H70"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="H70" sqref="H70"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.84375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.28515625" customWidth="1"/>
-    <col min="4" max="4" width="15.7109375" customWidth="1"/>
-    <col min="5" max="5" width="19.28515625" customWidth="1"/>
-    <col min="6" max="6" width="15.7109375" customWidth="1"/>
+    <col min="3" max="3" width="19.3046875" customWidth="1"/>
+    <col min="4" max="4" width="15.69140625" customWidth="1"/>
+    <col min="5" max="5" width="19.3046875" customWidth="1"/>
+    <col min="6" max="6" width="15.69140625" customWidth="1"/>
+    <col min="7" max="7" width="19.3046875" customWidth="1"/>
+    <col min="8" max="8" width="15.69140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -840,8 +848,14 @@
       <c r="F1" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1" t="s">
+        <v>145</v>
+      </c>
+      <c r="H1" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A2" s="1">
         <v>5110</v>
       </c>
@@ -860,8 +874,15 @@
       <c r="F2" s="4" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2" s="4" t="str">
+        <f>CONCATENATE(G2,"_")</f>
+        <v>01000_</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A3" s="1">
         <v>5121</v>
       </c>
@@ -880,8 +901,15 @@
       <c r="F3" s="4" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H3" s="4" t="str">
+        <f t="shared" ref="H3:H66" si="0">CONCATENATE(G3,"_")</f>
+        <v>02000_</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A4" s="1">
         <v>5122</v>
       </c>
@@ -900,8 +928,15 @@
       <c r="F4" s="4" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H4" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>03000_</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A5" s="1">
         <v>5131</v>
       </c>
@@ -920,8 +955,15 @@
       <c r="F5" s="4" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H5" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>06090_</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
@@ -940,8 +982,15 @@
       <c r="F6" s="4" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H6" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>10120_</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A7" s="1">
         <v>5150</v>
       </c>
@@ -960,8 +1009,15 @@
       <c r="F7" s="4" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G7" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H7" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>13150_</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A8" s="1" t="s">
         <v>4</v>
       </c>
@@ -980,8 +1036,15 @@
       <c r="F8" s="4" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G8" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H8" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>16000_</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C9" s="2" t="s">
         <v>14</v>
       </c>
@@ -994,8 +1057,15 @@
       <c r="F9" s="4" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G9" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H9" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>17000_</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C10" s="2" t="s">
         <v>15</v>
       </c>
@@ -1008,8 +1078,15 @@
       <c r="F10" s="4" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G10" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H10" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>18000_</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C11" s="2" t="s">
         <v>16</v>
       </c>
@@ -1022,8 +1099,15 @@
       <c r="F11" s="4" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G11" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H11" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>19000_</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C12" s="2" t="s">
         <v>17</v>
       </c>
@@ -1036,8 +1120,15 @@
       <c r="F12" s="4" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G12" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H12" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>20000_</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C13" s="2" t="s">
         <v>18</v>
       </c>
@@ -1050,8 +1141,15 @@
       <c r="F13" s="4" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G13" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H13" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>21000_</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C14" s="2" t="s">
         <v>19</v>
       </c>
@@ -1064,8 +1162,15 @@
       <c r="F14" s="4" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G14" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H14" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>22000_</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C15" s="2" t="s">
         <v>20</v>
       </c>
@@ -1078,8 +1183,15 @@
       <c r="F15" s="4" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G15" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H15" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>23000_</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.4">
       <c r="C16" s="2" t="s">
         <v>21</v>
       </c>
@@ -1092,8 +1204,15 @@
       <c r="F16" s="4" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="17" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="G16" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H16" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>24000_</v>
+      </c>
+    </row>
+    <row r="17" spans="3:8" x14ac:dyDescent="0.4">
       <c r="C17" s="2" t="s">
         <v>22</v>
       </c>
@@ -1106,8 +1225,15 @@
       <c r="F17" s="4" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="18" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="G17" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H17" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>25000_</v>
+      </c>
+    </row>
+    <row r="18" spans="3:8" x14ac:dyDescent="0.4">
       <c r="C18" s="2" t="s">
         <v>23</v>
       </c>
@@ -1120,8 +1246,15 @@
       <c r="F18" s="4" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="19" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="G18" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H18" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>26000_</v>
+      </c>
+    </row>
+    <row r="19" spans="3:8" x14ac:dyDescent="0.4">
       <c r="C19" s="2" t="s">
         <v>24</v>
       </c>
@@ -1134,8 +1267,15 @@
       <c r="F19" s="4" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="20" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="G19" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H19" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>27000_</v>
+      </c>
+    </row>
+    <row r="20" spans="3:8" x14ac:dyDescent="0.4">
       <c r="C20" s="2" t="s">
         <v>25</v>
       </c>
@@ -1148,8 +1288,15 @@
       <c r="F20" s="4" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="21" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="G20" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H20" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>28000_</v>
+      </c>
+    </row>
+    <row r="21" spans="3:8" x14ac:dyDescent="0.4">
       <c r="C21" s="2" t="s">
         <v>26</v>
       </c>
@@ -1162,8 +1309,15 @@
       <c r="F21" s="4" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="22" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="G21" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="H21" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>29000_</v>
+      </c>
+    </row>
+    <row r="22" spans="3:8" x14ac:dyDescent="0.4">
       <c r="C22" s="2" t="s">
         <v>27</v>
       </c>
@@ -1176,8 +1330,15 @@
       <c r="F22" s="4" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="23" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="G22" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="H22" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>30000_</v>
+      </c>
+    </row>
+    <row r="23" spans="3:8" x14ac:dyDescent="0.4">
       <c r="C23" s="2" t="s">
         <v>28</v>
       </c>
@@ -1190,8 +1351,15 @@
       <c r="F23" s="4" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="24" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="G23" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H23" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>31320_</v>
+      </c>
+    </row>
+    <row r="24" spans="3:8" x14ac:dyDescent="0.4">
       <c r="C24" s="2" t="s">
         <v>29</v>
       </c>
@@ -1204,8 +1372,15 @@
       <c r="F24" s="4" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="25" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="G24" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H24" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>33000_</v>
+      </c>
+    </row>
+    <row r="25" spans="3:8" x14ac:dyDescent="0.4">
       <c r="C25" s="2" t="s">
         <v>30</v>
       </c>
@@ -1218,8 +1393,15 @@
       <c r="F25" s="4" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="26" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="G25" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H25" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>35000_</v>
+      </c>
+    </row>
+    <row r="26" spans="3:8" x14ac:dyDescent="0.4">
       <c r="C26" s="2" t="s">
         <v>31</v>
       </c>
@@ -1232,8 +1414,15 @@
       <c r="F26" s="4" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="27" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="G26" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="H26" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>36000_</v>
+      </c>
+    </row>
+    <row r="27" spans="3:8" x14ac:dyDescent="0.4">
       <c r="C27" s="2" t="s">
         <v>32</v>
       </c>
@@ -1246,8 +1435,15 @@
       <c r="F27" s="4" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="28" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="G27" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="H27" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>37390_</v>
+      </c>
+    </row>
+    <row r="28" spans="3:8" x14ac:dyDescent="0.4">
       <c r="C28" s="2" t="s">
         <v>33</v>
       </c>
@@ -1260,8 +1456,15 @@
       <c r="F28" s="4" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="29" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="G28" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="H28" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>41430_</v>
+      </c>
+    </row>
+    <row r="29" spans="3:8" x14ac:dyDescent="0.4">
       <c r="C29" s="2" t="s">
         <v>34</v>
       </c>
@@ -1274,8 +1477,15 @@
       <c r="F29" s="4" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="30" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="G29" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="H29" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>45000_</v>
+      </c>
+    </row>
+    <row r="30" spans="3:8" x14ac:dyDescent="0.4">
       <c r="C30" s="2" t="s">
         <v>35</v>
       </c>
@@ -1288,8 +1498,15 @@
       <c r="F30" s="4" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="31" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="G30" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="H30" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>46000_</v>
+      </c>
+    </row>
+    <row r="31" spans="3:8" x14ac:dyDescent="0.4">
       <c r="C31" s="2" t="s">
         <v>36</v>
       </c>
@@ -1302,8 +1519,15 @@
       <c r="F31" s="4" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="32" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="G31" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="H31" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>47000_</v>
+      </c>
+    </row>
+    <row r="32" spans="3:8" x14ac:dyDescent="0.4">
       <c r="C32" s="2" t="s">
         <v>37</v>
       </c>
@@ -1316,8 +1540,15 @@
       <c r="F32" s="4" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="33" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="G32" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="H32" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>49000_</v>
+      </c>
+    </row>
+    <row r="33" spans="3:8" x14ac:dyDescent="0.4">
       <c r="C33" s="2" t="s">
         <v>38</v>
       </c>
@@ -1330,8 +1561,15 @@
       <c r="F33" s="4" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="34" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="G33" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="H33" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>50000_</v>
+      </c>
+    </row>
+    <row r="34" spans="3:8" x14ac:dyDescent="0.4">
       <c r="C34" s="2" t="s">
         <v>39</v>
       </c>
@@ -1344,8 +1582,15 @@
       <c r="F34" s="4" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="35" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="G34" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="H34" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>51000_</v>
+      </c>
+    </row>
+    <row r="35" spans="3:8" x14ac:dyDescent="0.4">
       <c r="C35" s="2" t="s">
         <v>40</v>
       </c>
@@ -1358,8 +1603,15 @@
       <c r="F35" s="4" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="36" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="G35" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="H35" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>52000_</v>
+      </c>
+    </row>
+    <row r="36" spans="3:8" x14ac:dyDescent="0.4">
       <c r="C36" s="2" t="s">
         <v>41</v>
       </c>
@@ -1372,8 +1624,15 @@
       <c r="F36" s="4" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="37" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="G36" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="H36" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>53000_</v>
+      </c>
+    </row>
+    <row r="37" spans="3:8" x14ac:dyDescent="0.4">
       <c r="C37" s="2" t="s">
         <v>42</v>
       </c>
@@ -1386,8 +1645,15 @@
       <c r="F37" s="4" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="38" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="G37" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="H37" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>55560_</v>
+      </c>
+    </row>
+    <row r="38" spans="3:8" x14ac:dyDescent="0.4">
       <c r="C38" s="2" t="s">
         <v>43</v>
       </c>
@@ -1400,8 +1666,15 @@
       <c r="F38" s="4" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="39" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="G38" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="H38" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>58000_</v>
+      </c>
+    </row>
+    <row r="39" spans="3:8" x14ac:dyDescent="0.4">
       <c r="C39" s="2" t="s">
         <v>44</v>
       </c>
@@ -1414,8 +1687,15 @@
       <c r="F39" s="4" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="40" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="G39" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="H39" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>59600_</v>
+      </c>
+    </row>
+    <row r="40" spans="3:8" x14ac:dyDescent="0.4">
       <c r="C40" s="2" t="s">
         <v>45</v>
       </c>
@@ -1428,8 +1708,15 @@
       <c r="F40" s="4" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="41" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="G40" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="H40" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>61000_</v>
+      </c>
+    </row>
+    <row r="41" spans="3:8" x14ac:dyDescent="0.4">
       <c r="C41" s="2" t="s">
         <v>46</v>
       </c>
@@ -1442,8 +1729,15 @@
       <c r="F41" s="4" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="42" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="G41" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="H41" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>62630_</v>
+      </c>
+    </row>
+    <row r="42" spans="3:8" x14ac:dyDescent="0.4">
       <c r="C42" s="2" t="s">
         <v>47</v>
       </c>
@@ -1456,8 +1750,15 @@
       <c r="F42" s="4" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="43" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="G42" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="H42" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>64000_</v>
+      </c>
+    </row>
+    <row r="43" spans="3:8" x14ac:dyDescent="0.4">
       <c r="C43" s="2" t="s">
         <v>48</v>
       </c>
@@ -1470,8 +1771,15 @@
       <c r="F43" s="4" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="44" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="G43" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="H43" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>65000_</v>
+      </c>
+    </row>
+    <row r="44" spans="3:8" x14ac:dyDescent="0.4">
       <c r="C44" s="2" t="s">
         <v>49</v>
       </c>
@@ -1484,8 +1792,15 @@
       <c r="F44" s="4" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="45" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="G44" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="H44" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>66000_</v>
+      </c>
+    </row>
+    <row r="45" spans="3:8" x14ac:dyDescent="0.4">
       <c r="C45" s="2" t="s">
         <v>50</v>
       </c>
@@ -1498,8 +1813,15 @@
       <c r="F45" s="4" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="46" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="G45" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="H45" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>68100_</v>
+      </c>
+    </row>
+    <row r="46" spans="3:8" x14ac:dyDescent="0.4">
       <c r="C46" s="2" t="s">
         <v>51</v>
       </c>
@@ -1512,8 +1834,15 @@
       <c r="F46" s="4" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="47" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="G46" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="H46" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>68300_</v>
+      </c>
+    </row>
+    <row r="47" spans="3:8" x14ac:dyDescent="0.4">
       <c r="C47" s="2" t="s">
         <v>52</v>
       </c>
@@ -1526,8 +1855,15 @@
       <c r="F47" s="4" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="48" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="G47" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="H47" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>68203_</v>
+      </c>
+    </row>
+    <row r="48" spans="3:8" x14ac:dyDescent="0.4">
       <c r="C48" s="2" t="s">
         <v>53</v>
       </c>
@@ -1540,8 +1876,15 @@
       <c r="F48" s="4" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="49" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="G48" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="H48" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>68204_</v>
+      </c>
+    </row>
+    <row r="49" spans="3:8" x14ac:dyDescent="0.4">
       <c r="C49" s="2" t="s">
         <v>54</v>
       </c>
@@ -1554,8 +1897,15 @@
       <c r="F49" s="4" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="50" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="G49" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="H49" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>69700_</v>
+      </c>
+    </row>
+    <row r="50" spans="3:8" x14ac:dyDescent="0.4">
       <c r="C50" s="2" t="s">
         <v>55</v>
       </c>
@@ -1568,8 +1918,15 @@
       <c r="F50" s="4" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="51" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="G50" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="H50" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>71000_</v>
+      </c>
+    </row>
+    <row r="51" spans="3:8" x14ac:dyDescent="0.4">
       <c r="C51" s="2" t="s">
         <v>56</v>
       </c>
@@ -1582,8 +1939,15 @@
       <c r="F51" s="4" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="52" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="G51" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="H51" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>72001_</v>
+      </c>
+    </row>
+    <row r="52" spans="3:8" x14ac:dyDescent="0.4">
       <c r="C52" s="2" t="s">
         <v>57</v>
       </c>
@@ -1596,8 +1960,15 @@
       <c r="F52" s="4" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="53" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="G52" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="H52" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>72002_</v>
+      </c>
+    </row>
+    <row r="53" spans="3:8" x14ac:dyDescent="0.4">
       <c r="C53" s="2" t="s">
         <v>58</v>
       </c>
@@ -1610,8 +1981,15 @@
       <c r="F53" s="4" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="54" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="G53" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="H53" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>73000_</v>
+      </c>
+    </row>
+    <row r="54" spans="3:8" x14ac:dyDescent="0.4">
       <c r="C54" s="2" t="s">
         <v>59</v>
       </c>
@@ -1624,8 +2002,15 @@
       <c r="F54" s="4" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="55" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="G54" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="H54" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>74750_</v>
+      </c>
+    </row>
+    <row r="55" spans="3:8" x14ac:dyDescent="0.4">
       <c r="C55" s="2" t="s">
         <v>60</v>
       </c>
@@ -1638,8 +2023,15 @@
       <c r="F55" s="4" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="56" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="G55" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="H55" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>77000_</v>
+      </c>
+    </row>
+    <row r="56" spans="3:8" x14ac:dyDescent="0.4">
       <c r="C56" s="2" t="s">
         <v>61</v>
       </c>
@@ -1652,8 +2044,15 @@
       <c r="F56" s="4" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="57" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="G56" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="H56" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>78000_</v>
+      </c>
+    </row>
+    <row r="57" spans="3:8" x14ac:dyDescent="0.4">
       <c r="C57" s="2" t="s">
         <v>62</v>
       </c>
@@ -1666,8 +2065,15 @@
       <c r="F57" s="4" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="58" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="G57" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="H57" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>79000_</v>
+      </c>
+    </row>
+    <row r="58" spans="3:8" x14ac:dyDescent="0.4">
       <c r="C58" s="2" t="s">
         <v>63</v>
       </c>
@@ -1680,8 +2086,15 @@
       <c r="F58" s="4" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="59" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="G58" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="H58" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>80820_</v>
+      </c>
+    </row>
+    <row r="59" spans="3:8" x14ac:dyDescent="0.4">
       <c r="C59" s="2" t="s">
         <v>64</v>
       </c>
@@ -1694,8 +2107,15 @@
       <c r="F59" s="4" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="60" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="G59" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="H59" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>84202_</v>
+      </c>
+    </row>
+    <row r="60" spans="3:8" x14ac:dyDescent="0.4">
       <c r="C60" s="2" t="s">
         <v>65</v>
       </c>
@@ -1708,8 +2128,15 @@
       <c r="F60" s="4" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="61" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="G60" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="H60" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>84101_</v>
+      </c>
+    </row>
+    <row r="61" spans="3:8" x14ac:dyDescent="0.4">
       <c r="C61" s="2" t="s">
         <v>66</v>
       </c>
@@ -1722,8 +2149,15 @@
       <c r="F61" s="4" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="62" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="G61" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="H61" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>85202_</v>
+      </c>
+    </row>
+    <row r="62" spans="3:8" x14ac:dyDescent="0.4">
       <c r="C62" s="2" t="s">
         <v>67</v>
       </c>
@@ -1736,8 +2170,15 @@
       <c r="F62" s="4" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="63" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="G62" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="H62" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>85101_</v>
+      </c>
+    </row>
+    <row r="63" spans="3:8" x14ac:dyDescent="0.4">
       <c r="C63" s="2" t="s">
         <v>68</v>
       </c>
@@ -1750,8 +2191,15 @@
       <c r="F63" s="4" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="64" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="G63" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="H63" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>86000_</v>
+      </c>
+    </row>
+    <row r="64" spans="3:8" x14ac:dyDescent="0.4">
       <c r="C64" s="2" t="s">
         <v>69</v>
       </c>
@@ -1764,8 +2212,15 @@
       <c r="F64" s="4" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="65" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="G64" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="H64" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>87880_</v>
+      </c>
+    </row>
+    <row r="65" spans="3:8" x14ac:dyDescent="0.4">
       <c r="C65" s="2" t="s">
         <v>70</v>
       </c>
@@ -1778,8 +2233,15 @@
       <c r="F65" s="4" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="66" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="G65" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="H65" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>90920_</v>
+      </c>
+    </row>
+    <row r="66" spans="3:8" x14ac:dyDescent="0.4">
       <c r="C66" s="2" t="s">
         <v>71</v>
       </c>
@@ -1792,8 +2254,15 @@
       <c r="F66" s="4" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="67" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="G66" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="H66" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>93000_</v>
+      </c>
+    </row>
+    <row r="67" spans="3:8" x14ac:dyDescent="0.4">
       <c r="C67" s="2" t="s">
         <v>72</v>
       </c>
@@ -1806,8 +2275,15 @@
       <c r="F67" s="4" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="68" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="G67" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="H67" s="4" t="str">
+        <f t="shared" ref="H67:H70" si="1">CONCATENATE(G67,"_")</f>
+        <v>94000_</v>
+      </c>
+    </row>
+    <row r="68" spans="3:8" x14ac:dyDescent="0.4">
       <c r="C68" s="2" t="s">
         <v>73</v>
       </c>
@@ -1820,8 +2296,15 @@
       <c r="F68" s="4" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="69" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="G68" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="H68" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>95000_</v>
+      </c>
+    </row>
+    <row r="69" spans="3:8" x14ac:dyDescent="0.4">
       <c r="C69" s="2" t="s">
         <v>10</v>
       </c>
@@ -1834,8 +2317,15 @@
       <c r="F69" s="4" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="70" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="G69" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H69" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>96000_</v>
+      </c>
+    </row>
+    <row r="70" spans="3:8" x14ac:dyDescent="0.4">
       <c r="C70" s="3" t="s">
         <v>74</v>
       </c>
@@ -1847,6 +2337,12 @@
       </c>
       <c r="F70" s="4" t="s">
         <v>82</v>
+      </c>
+      <c r="G70" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="H70" s="4" t="s">
+        <v>143</v>
       </c>
     </row>
   </sheetData>

</xml_diff>